<commit_message>
fix some magician card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spike.xlsx
+++ b/ConfigData/Xlsx/Spike.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -42,14 +42,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>魔法变化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>领导变化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>MpCostChange</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -141,6 +133,18 @@
   </si>
   <si>
     <t>回合持续</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>巫师学徒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LP变化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MP变化</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1243,8 +1247,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:I10" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="A3:I10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:I11" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A3:I11"/>
   <sortState ref="A4:Z126">
     <sortCondition ref="A3:A126"/>
   </sortState>
@@ -1550,13 +1554,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1574,25 +1578,25 @@
         <v>4</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>24</v>
-      </c>
       <c r="I1" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1612,45 +1616,45 @@
         <v>5</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>10</v>
-      </c>
       <c r="F3" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1658,7 +1662,7 @@
         <v>57000001</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="7">
         <v>3</v>
@@ -1673,13 +1677,13 @@
         <v>0</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1687,7 +1691,7 @@
         <v>57000002</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="7">
         <v>-3</v>
@@ -1702,13 +1706,13 @@
         <v>0</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1716,7 +1720,7 @@
         <v>57000003</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
@@ -1731,13 +1735,13 @@
         <v>0</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1745,7 +1749,7 @@
         <v>57000004</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
@@ -1760,13 +1764,13 @@
         <v>0</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1774,7 +1778,7 @@
         <v>57000005</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="7">
         <v>0</v>
@@ -1789,13 +1793,13 @@
         <v>0</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1803,7 +1807,7 @@
         <v>57000006</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
@@ -1818,13 +1822,13 @@
         <v>0</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1832,7 +1836,7 @@
         <v>57000007</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
@@ -1847,13 +1851,42 @@
         <v>1</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="7">
+        <v>57000008</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="7">
+        <v>-1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="19">
+        <v>0</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="13" t="s">
-        <v>25</v>
+      <c r="H11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish the card mommy
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spike.xlsx
+++ b/ConfigData/Xlsx/Spike.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -1560,7 +1560,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
remake the spike gather effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spike.xlsx
+++ b/ConfigData/Xlsx/Spike.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -88,63 +88,91 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用怪物卡后消失</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用武器消失</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命之力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>洛布</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Round</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合持续</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>巫师学徒</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LP变化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MP变化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>特殊效果</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tag</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用魔法消失</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>RemoveOnUseWeapon</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>bool</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用怪物卡后消失</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用武器消失</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用魔法消失</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>生命之力</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>洛布</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Round</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>float</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合持续</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>巫师学徒</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>LP变化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>MP变化</t>
+    <t>集结</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>doublecard</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>禁忌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mirrorspell</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -339,7 +367,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,6 +586,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -837,7 +877,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -868,9 +908,6 @@
     <xf numFmtId="0" fontId="21" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -896,6 +933,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -943,7 +986,30 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1247,21 +1313,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:I11" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="A3:I11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:J13" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A3:J13"/>
   <sortState ref="A4:Z126">
     <sortCondition ref="A3:A126"/>
   </sortState>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Id" dataDxfId="8"/>
-    <tableColumn id="2" name="Name" dataDxfId="7"/>
-    <tableColumn id="3" name="MpCostChange" dataDxfId="6"/>
-    <tableColumn id="4" name="LpCostChange" dataDxfId="5"/>
-    <tableColumn id="5" name="PpCostChange" dataDxfId="4"/>
-    <tableColumn id="9" name="Round" dataDxfId="3"/>
-    <tableColumn id="6" name="RemoveOnUseMonster" dataDxfId="2"/>
-    <tableColumn id="7" name="RemoveOnUseSpell" dataDxfId="1"/>
-    <tableColumn id="8" name="RemoveOnUseWeapon" dataDxfId="0"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Id" dataDxfId="9"/>
+    <tableColumn id="2" name="Name" dataDxfId="8"/>
+    <tableColumn id="3" name="MpCostChange" dataDxfId="7"/>
+    <tableColumn id="4" name="LpCostChange" dataDxfId="6"/>
+    <tableColumn id="5" name="PpCostChange" dataDxfId="5"/>
+    <tableColumn id="10" name="Tag" dataDxfId="0"/>
+    <tableColumn id="9" name="Round" dataDxfId="4"/>
+    <tableColumn id="6" name="RemoveOnUseMonster" dataDxfId="3"/>
+    <tableColumn id="7" name="RemoveOnUseSpell" dataDxfId="2"/>
+    <tableColumn id="8" name="RemoveOnUseWeapon" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1554,23 +1621,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.75" customWidth="1"/>
-    <col min="2" max="2" width="7.875" customWidth="1"/>
-    <col min="3" max="6" width="5.375" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" customWidth="1"/>
+    <col min="3" max="5" width="5.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="65.25" customHeight="1">
+    <row r="1" spans="1:10" ht="65.25" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -1578,28 +1647,31 @@
         <v>4</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1609,26 +1681,29 @@
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>19</v>
+      <c r="F2" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1644,20 +1719,23 @@
       <c r="E3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>18</v>
+      <c r="J3" s="17" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="4">
         <v>57000001</v>
       </c>
@@ -1673,20 +1751,21 @@
       <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="F4" s="19">
-        <v>0</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>23</v>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18">
+        <v>0</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="4">
         <v>57000002</v>
       </c>
@@ -1702,20 +1781,21 @@
       <c r="E5" s="7">
         <v>0</v>
       </c>
-      <c r="F5" s="19">
-        <v>0</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>23</v>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="4">
         <v>57000003</v>
       </c>
@@ -1731,20 +1811,21 @@
       <c r="E6" s="7">
         <v>0</v>
       </c>
-      <c r="F6" s="19">
-        <v>0</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>23</v>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18">
+        <v>0</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="4">
         <v>57000004</v>
       </c>
@@ -1760,20 +1841,21 @@
       <c r="E7" s="7">
         <v>1</v>
       </c>
-      <c r="F7" s="19">
-        <v>0</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>23</v>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="4">
         <v>57000005</v>
       </c>
@@ -1789,25 +1871,26 @@
       <c r="E8" s="7">
         <v>-2</v>
       </c>
-      <c r="F8" s="19">
-        <v>0</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>23</v>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="4">
         <v>57000006</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="7">
         <v>0</v>
@@ -1818,25 +1901,26 @@
       <c r="E9" s="7">
         <v>0</v>
       </c>
-      <c r="F9" s="19">
-        <v>0</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="13" t="s">
+      <c r="F9" s="18"/>
+      <c r="G9" s="18">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="13" t="s">
-        <v>23</v>
+      <c r="I9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="7">
         <v>57000007</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
@@ -1847,25 +1931,26 @@
       <c r="E10" s="7">
         <v>0</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="18"/>
+      <c r="G10" s="18">
         <v>1</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="13" t="s">
-        <v>23</v>
+      <c r="I10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="7">
         <v>57000008</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="7">
         <v>-1</v>
@@ -1876,17 +1961,82 @@
       <c r="E11" s="7">
         <v>0</v>
       </c>
-      <c r="F11" s="19">
-        <v>0</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="13" t="s">
+      <c r="F11" s="18"/>
+      <c r="G11" s="18">
+        <v>0</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="13" t="s">
-        <v>23</v>
+      <c r="I11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="7">
+        <v>57000009</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="18">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="7">
+        <v>57000010</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="18">
+        <v>0</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fnish some monster card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Spike.xlsx
+++ b/ConfigData/Xlsx/Spike.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -173,6 +173,14 @@
   </si>
   <si>
     <t>mirrorspell</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lp2mp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>远古龙</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1003,6 +1011,7 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1074,7 +1083,6 @@
         <name val="宋体"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1313,8 +1321,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:J13" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="A3:J13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:J14" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A3:J14"/>
   <sortState ref="A4:Z126">
     <sortCondition ref="A3:A126"/>
   </sortState>
@@ -1324,11 +1332,11 @@
     <tableColumn id="3" name="MpCostChange" dataDxfId="7"/>
     <tableColumn id="4" name="LpCostChange" dataDxfId="6"/>
     <tableColumn id="5" name="PpCostChange" dataDxfId="5"/>
-    <tableColumn id="10" name="Tag" dataDxfId="0"/>
-    <tableColumn id="9" name="Round" dataDxfId="4"/>
-    <tableColumn id="6" name="RemoveOnUseMonster" dataDxfId="3"/>
-    <tableColumn id="7" name="RemoveOnUseSpell" dataDxfId="2"/>
-    <tableColumn id="8" name="RemoveOnUseWeapon" dataDxfId="1"/>
+    <tableColumn id="10" name="Tag" dataDxfId="4"/>
+    <tableColumn id="9" name="Round" dataDxfId="3"/>
+    <tableColumn id="6" name="RemoveOnUseMonster" dataDxfId="2"/>
+    <tableColumn id="7" name="RemoveOnUseSpell" dataDxfId="1"/>
+    <tableColumn id="8" name="RemoveOnUseWeapon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1621,13 +1629,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2039,6 +2047,38 @@
         <v>21</v>
       </c>
     </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="7">
+        <v>57000011</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="18">
+        <v>0</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>